<commit_message>
Milestone #1 GUI Updated
</commit_message>
<xml_diff>
--- a/201213018-WBS.xlsx
+++ b/201213018-WBS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrakd\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrakd\Desktop\Depository\flutter_projects\sensor_box\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D744AEDC-2DC7-4C46-A979-5F91A9F81155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C019E61-7275-41C0-8B9C-17F0B4BB6C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B772B289-56D3-41E8-8789-9F94D0B1FB09}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Final Haftası</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Uygulamadaki tasarım hatalarının giderilmesi</t>
   </si>
   <si>
-    <t>Uygulamadaki backend hatalarının giderilmesi</t>
-  </si>
-  <si>
     <t>Sensör verilerinin uygun bir şekilde saklanabilmesi için gerekli veritabanının oluşturulması</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
   </si>
   <si>
     <t>Bitti</t>
-  </si>
-  <si>
-    <t>Devam Ediyor</t>
   </si>
   <si>
     <t>Başlamadı</t>
@@ -303,48 +297,48 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,38 +671,38 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="76.88671875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="76.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -717,326 +711,326 @@
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4" s="3">
         <v>44987</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>40</v>
+      <c r="D4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
       <c r="B5" s="3">
         <v>44994</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>40</v>
+      <c r="E5" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
       <c r="B6" s="3">
         <v>45001</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>41</v>
+      <c r="E6" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
       <c r="B7" s="3">
         <v>45008</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>42</v>
+      <c r="E7" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>45015</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>42</v>
+      <c r="E8" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>45022</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>42</v>
+      <c r="E9" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
       <c r="B10" s="3">
         <v>45029</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>42</v>
+      <c r="E10" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
       <c r="B11" s="3">
         <v>45036</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>42</v>
+      <c r="D11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="A12" s="4">
         <v>9</v>
       </c>
       <c r="B12" s="3">
         <v>45043</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>42</v>
+      <c r="D12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>45050</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="19" t="s">
-        <v>42</v>
+      <c r="D13" s="9"/>
+      <c r="E13" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+      <c r="A14" s="4">
         <v>11</v>
       </c>
       <c r="B14" s="3">
         <v>45057</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>42</v>
+      <c r="E14" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="A15" s="4">
         <v>12</v>
       </c>
       <c r="B15" s="3">
         <v>45064</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>42</v>
+      <c r="E15" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="A16" s="4">
         <v>13</v>
       </c>
       <c r="B16" s="3">
         <v>45071</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>42</v>
+      <c r="D16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="A17" s="4">
         <v>14</v>
       </c>
       <c r="B17" s="3">
         <v>45078</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>42</v>
+      <c r="E17" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+      <c r="A18" s="4">
         <v>15</v>
       </c>
       <c r="B18" s="3">
         <v>45085</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>42</v>
+      <c r="E18" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="A19" s="4">
         <v>16</v>
       </c>
       <c r="B19" s="3">
         <v>45092</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="19" t="s">
-        <v>42</v>
+      <c r="D19" s="9"/>
+      <c r="E19" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="A20" s="4">
         <v>17</v>
       </c>
       <c r="B20" s="3">
         <v>45099</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="19" t="s">
-        <v>42</v>
+      <c r="D20" s="9"/>
+      <c r="E20" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="A21" s="4">
         <v>18</v>
       </c>
       <c r="B21" s="3">
         <v>45106</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>42</v>
+      <c r="C21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="A22" s="4">
         <v>19</v>
       </c>
       <c r="B22" s="3">
         <v>45113</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="19" t="s">
-        <v>42</v>
+      <c r="D22" s="9"/>
+      <c r="E22" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>